<commit_message>
Added 2022 Bar Plots
</commit_message>
<xml_diff>
--- a/dps_dashboard/data/2020/school_stats_data/poc per school22.xlsx
+++ b/dps_dashboard/data/2020/school_stats_data/poc per school22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melaniemoseley/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scholar/CodingWorkspace/visualizing_DPS/dps_dashboard/data/2020/school_stats_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE17CEFA-539F-A24B-A98D-2577FBCDC6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434058DE-DD95-3E4F-BE6F-BA5CF1162686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1100" windowWidth="27640" windowHeight="15640" xr2:uid="{8A77730F-63B3-7A4A-B171-15DB83AB20AC}"/>
+    <workbookView xWindow="7360" yWindow="1020" windowWidth="27640" windowHeight="15640" xr2:uid="{8A77730F-63B3-7A4A-B171-15DB83AB20AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>place</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>E.K. Powe Elementary</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -468,7 +465,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,8 +567,8 @@
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
+      <c r="B12" s="1">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>